<commit_message>
implement all the logic
</commit_message>
<xml_diff>
--- a/attributes.xlsx
+++ b/attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariisichoix/art-engine-py/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1101312B-3E98-B940-8D0B-0EB0AACC61DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB417234-A035-F749-99C8-915B14CC565A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20600" yWindow="-21100" windowWidth="28040" windowHeight="17440" xr2:uid="{2853084E-1E11-FC43-A58D-24800EBC98CF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19980" xr2:uid="{2853084E-1E11-FC43-A58D-24800EBC98CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="492">
   <si>
     <t>GROUPS</t>
   </si>
@@ -1499,6 +1499,18 @@
   </si>
   <si>
     <t>MEXICAN</t>
+  </si>
+  <si>
+    <t>DAGGER RUSTED MOUTH</t>
+  </si>
+  <si>
+    <t>DAGGER BLACK MOUTH</t>
+  </si>
+  <si>
+    <t>DAGGER GOLD JRS MOUTH</t>
+  </si>
+  <si>
+    <t>GOLD TEETH</t>
   </si>
 </sst>
 </file>
@@ -1891,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53E7DC0-4282-3A47-9194-E315E41B58F0}">
   <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1961,7 +1973,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
@@ -2321,7 +2333,7 @@
         <v>73</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>33</v>
+        <v>491</v>
       </c>
       <c r="D32" s="2">
         <v>0.1</v>
@@ -3826,7 +3838,7 @@
         <v>286</v>
       </c>
       <c r="D138" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>82</v>
@@ -4862,7 +4874,7 @@
         <v>430</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>313</v>
+        <v>488</v>
       </c>
       <c r="D212" s="2">
         <v>3</v>
@@ -4876,7 +4888,7 @@
         <v>431</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>315</v>
+        <v>489</v>
       </c>
       <c r="D213" s="2">
         <v>3</v>
@@ -4890,7 +4902,7 @@
         <v>432</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>317</v>
+        <v>490</v>
       </c>
       <c r="D214" s="2">
         <v>1</v>

</xml_diff>